<commit_message>
add test for c_pi_open
</commit_message>
<xml_diff>
--- a/utilityscripts/wind/as1170_2_data.xlsx
+++ b/utilityscripts/wind/as1170_2_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\wind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4865C575-8BD6-4DFB-AA52-9AF05500E3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2105AF-D241-47A7-A450-04C8B5CDEAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wind_direction_definitions" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="69">
   <si>
     <t>N</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>AS/NZS1170.2-2021</t>
+  </si>
+  <si>
+    <t>consider_c_pe</t>
   </si>
 </sst>
 </file>
@@ -7190,16 +7193,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{773ABC32-8E46-4EEC-8415-C11FEF17412F}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -7215,7 +7218,7 @@
         <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
         <v>48</v>
@@ -7633,7 +7636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9FBCEA-2FDF-421C-9250-63381978FDC5}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
as1170.2 add c_pe_l method.
</commit_message>
<xml_diff>
--- a/utilityscripts/wind/as1170_2_data.xlsx
+++ b/utilityscripts/wind/as1170_2_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\wind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2105AF-D241-47A7-A450-04C8B5CDEAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2444D73-BFCE-4AAC-846E-74D18BD9DD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wind_direction_definitions" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,9 @@
     <sheet name="cpi_t5a" sheetId="7" r:id="rId6"/>
     <sheet name="cpi_t5b" sheetId="8" r:id="rId7"/>
     <sheet name="k_a" sheetId="9" r:id="rId8"/>
-    <sheet name="cpe_t5_2c" sheetId="10" r:id="rId9"/>
-    <sheet name="app_c_fig_c2" sheetId="11" r:id="rId10"/>
+    <sheet name="cpe_t5_2b" sheetId="12" r:id="rId9"/>
+    <sheet name="cpe_t5_2c" sheetId="10" r:id="rId10"/>
+    <sheet name="app_c_fig_c2" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="73">
   <si>
     <t>N</t>
   </si>
@@ -249,6 +250,18 @@
   </si>
   <si>
     <t>consider_c_pe</t>
+  </si>
+  <si>
+    <t>hip_or_gable</t>
+  </si>
+  <si>
+    <t>hip</t>
+  </si>
+  <si>
+    <t>gable</t>
+  </si>
+  <si>
+    <t>roof_pitch</t>
   </si>
 </sst>
 </file>
@@ -689,6 +702,102 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02C147CC-3A12-402B-BB71-F03DBCCD8C15}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>-0.65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="C3">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5">
+        <v>2.0009999999999999</v>
+      </c>
+      <c r="C5">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7">
+        <v>3.0009999999999999</v>
+      </c>
+      <c r="C7">
+        <v>-0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D6BFCE-8807-4FA6-8CAD-90A0E49EBC9F}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -7193,7 +7302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{773ABC32-8E46-4EEC-8415-C11FEF17412F}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -7978,93 +8087,1107 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02C147CC-3A12-402B-BB71-F03DBCCD8C15}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BA6DCA-9FF6-4DD9-8B4A-BF73F318CE2D}">
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>70</v>
       </c>
       <c r="C2">
-        <v>-0.65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
-      <c r="B3">
-        <v>1.0009999999999999</v>
+      <c r="B3" t="s">
+        <v>70</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3">
         <v>-0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0.3</v>
+      </c>
+      <c r="E4">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="E6">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1000</v>
+      </c>
+      <c r="E8">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9">
+        <v>9.9999000000000002</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>-0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5">
-        <v>2.0009999999999999</v>
-      </c>
-      <c r="C5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10">
+        <v>9.9999000000000002</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+      <c r="E10">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11">
+        <v>9.9999000000000002</v>
+      </c>
+      <c r="D11">
+        <v>0.3</v>
+      </c>
+      <c r="E11">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12">
+        <v>9.9999000000000002</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13">
+        <v>9.9999000000000002</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
         <v>-0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14">
+        <v>9.9999000000000002</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15">
+        <v>9.9999000000000002</v>
+      </c>
+      <c r="D15">
+        <v>1000</v>
+      </c>
+      <c r="E15">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <v>-0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7">
-        <v>3.0009999999999999</v>
-      </c>
-      <c r="C7">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+      <c r="E17">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>0.3</v>
+      </c>
+      <c r="E18">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>1000</v>
+      </c>
+      <c r="E22">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24">
+        <v>15</v>
+      </c>
+      <c r="D24">
+        <v>0.1</v>
+      </c>
+      <c r="E24">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25">
+        <v>15</v>
+      </c>
+      <c r="D25">
+        <v>0.3</v>
+      </c>
+      <c r="E25">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27">
+        <v>15</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29">
+        <v>15</v>
+      </c>
+      <c r="D29">
+        <v>1000</v>
+      </c>
+      <c r="E29">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30">
+        <v>20</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31">
+        <v>20</v>
+      </c>
+      <c r="D31">
+        <v>0.1</v>
+      </c>
+      <c r="E31">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32">
+        <v>20</v>
+      </c>
+      <c r="D32">
+        <v>0.3</v>
+      </c>
+      <c r="E32">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33">
+        <v>20</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34">
+        <v>20</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35">
+        <v>20</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36">
+        <v>20</v>
+      </c>
+      <c r="D36">
+        <v>1000</v>
+      </c>
+      <c r="E36">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37">
+        <v>25</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>-0.75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38">
+        <v>25</v>
+      </c>
+      <c r="D38">
+        <v>0.1</v>
+      </c>
+      <c r="E38">
+        <v>-0.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39">
+        <v>25</v>
+      </c>
+      <c r="D39">
+        <v>0.3</v>
+      </c>
+      <c r="E39">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40">
+        <v>25</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41">
+        <v>25</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42">
+        <v>25</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43">
+        <v>25</v>
+      </c>
+      <c r="D43">
+        <v>1000</v>
+      </c>
+      <c r="E43">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44">
+        <v>90</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>-0.75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45">
+        <v>90</v>
+      </c>
+      <c r="D45">
+        <v>0.1</v>
+      </c>
+      <c r="E45">
+        <v>-0.75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46">
+        <v>90</v>
+      </c>
+      <c r="D46">
+        <v>0.3</v>
+      </c>
+      <c r="E46">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47">
+        <v>90</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48">
+        <v>90</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49">
+        <v>90</v>
+      </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+      <c r="E49">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50">
+        <v>90</v>
+      </c>
+      <c r="D50">
+        <v>1000</v>
+      </c>
+      <c r="E50">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0.1</v>
+      </c>
+      <c r="E52">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0.3</v>
+      </c>
+      <c r="E53">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>4</v>
+      </c>
+      <c r="E56">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>67</v>
+      </c>
+      <c r="B57" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>1000</v>
+      </c>
+      <c r="E57">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58">
+        <v>90</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59">
+        <v>90</v>
+      </c>
+      <c r="D59">
+        <v>0.1</v>
+      </c>
+      <c r="E59">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" t="s">
+        <v>71</v>
+      </c>
+      <c r="C60">
+        <v>90</v>
+      </c>
+      <c r="D60">
+        <v>0.3</v>
+      </c>
+      <c r="E60">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" t="s">
+        <v>71</v>
+      </c>
+      <c r="C61">
+        <v>90</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62">
+        <v>90</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63">
+        <v>90</v>
+      </c>
+      <c r="D63">
+        <v>4</v>
+      </c>
+      <c r="E63">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64">
+        <v>90</v>
+      </c>
+      <c r="D64">
+        <v>1000</v>
+      </c>
+      <c r="E64">
         <v>-0.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add open section aspect ratio factor k_ar.
</commit_message>
<xml_diff>
--- a/utilityscripts/wind/as1170_2_data.xlsx
+++ b/utilityscripts/wind/as1170_2_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\wind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2444D73-BFCE-4AAC-846E-74D18BD9DD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E2741E-C6FF-40BE-9D8E-4530F7FE4100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wind_direction_definitions" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,8 @@
     <sheet name="k_a" sheetId="9" r:id="rId8"/>
     <sheet name="cpe_t5_2b" sheetId="12" r:id="rId9"/>
     <sheet name="cpe_t5_2c" sheetId="10" r:id="rId10"/>
-    <sheet name="app_c_fig_c2" sheetId="11" r:id="rId11"/>
+    <sheet name="app_c_k_ar" sheetId="13" r:id="rId11"/>
+    <sheet name="app_c_fig_c2" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="75">
   <si>
     <t>N</t>
   </si>
@@ -262,6 +263,12 @@
   </si>
   <si>
     <t>roof_pitch</t>
+  </si>
+  <si>
+    <t>l_b_ratio</t>
+  </si>
+  <si>
+    <t>k_ar</t>
   </si>
 </sst>
 </file>
@@ -798,6 +805,77 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CD81D0-55A7-4456-A3DB-308C17548CC0}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1000</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D6BFCE-8807-4FA6-8CAD-90A0E49EBC9F}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -8090,7 +8168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BA6DCA-9FF6-4DD9-8B4A-BF73F318CE2D}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>

</xml_diff>